<commit_message>
fix wrong round trips rename traveldata to missionsdata put missiondata in emissioncalculator
</commit_message>
<xml_diff>
--- a/Data/Raw/MIS_2022_extrait.xlsx
+++ b/Data/Raw/MIS_2022_extrait.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="2022" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="2022" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -200,12 +200,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -221,312 +225,418 @@
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="LibreOffice">
+      <a:dk1>
+        <a:srgbClr val="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:srgbClr val="ffffff"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="000000"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="ffffff"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="18a303"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="0369a3"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="a33e03"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8e03a3"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="c99c00"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="c9211e"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000ee"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="551a8b"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme>
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
+      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="22.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="17.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="30.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="9.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="12.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="25.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="11.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="14.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="13.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="22.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="13.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="16.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="17.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="30.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="9.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="12.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="25.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="11.43"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="0" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
+      <c r="A2" s="1" t="n">
         <v>7959</v>
       </c>
-      <c r="B2" s="1" t="n">
+      <c r="B2" s="2" t="n">
         <v>44585</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" s="0" t="s">
+      <c r="D2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" s="0" t="s">
+      <c r="F2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="0" t="s">
+      <c r="I2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="J2" s="0" t="s">
+      <c r="J2" s="1" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
+      <c r="A3" s="1" t="n">
         <v>7960</v>
       </c>
-      <c r="B3" s="1" t="n">
+      <c r="B3" s="2" t="n">
         <v>44585</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="0" t="s">
+      <c r="D3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" s="0" t="s">
+      <c r="F3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="0" t="s">
+      <c r="I3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="J3" s="0" t="s">
+      <c r="J3" s="1" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
+      <c r="A4" s="1" t="n">
         <v>7961</v>
       </c>
-      <c r="B4" s="1" t="n">
+      <c r="B4" s="2" t="n">
         <v>44585</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" s="0" t="s">
+      <c r="D4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="G4" s="0" t="s">
+      <c r="F4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="I4" s="0" t="s">
+      <c r="I4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="J4" s="0" t="s">
+      <c r="J4" s="1" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
+      <c r="A5" s="1" t="n">
         <v>7963</v>
       </c>
-      <c r="B5" s="1" t="n">
+      <c r="B5" s="2" t="n">
         <v>44578</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="0" t="s">
+      <c r="D5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F5" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="G5" s="0" t="s">
+      <c r="F5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="H5" s="0" t="n">
+      <c r="H5" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="I5" s="0" t="s">
+      <c r="I5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="0" t="s">
+      <c r="J5" s="1" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="n">
+      <c r="A6" s="1" t="n">
         <v>7967</v>
       </c>
-      <c r="B6" s="1" t="n">
+      <c r="B6" s="2" t="n">
         <v>44578</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" s="0" t="s">
+      <c r="D6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F6" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="G6" s="0" t="s">
+      <c r="F6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="H6" s="0" t="n">
+      <c r="H6" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="I6" s="0" t="s">
+      <c r="I6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="J6" s="0" t="s">
+      <c r="J6" s="1" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="n">
+      <c r="A7" s="1" t="n">
         <v>7975</v>
       </c>
-      <c r="B7" s="1" t="n">
+      <c r="B7" s="2" t="n">
         <v>44582</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C7" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" s="0" t="s">
+      <c r="D7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F7" s="0" t="s">
+      <c r="F7" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="I7" s="0" t="s">
+      <c r="I7" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="J7" s="0" t="s">
+      <c r="J7" s="1" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="n">
-        <v>7976</v>
-      </c>
-      <c r="B8" s="1" t="n">
+      <c r="A8" s="1" t="n">
+        <v>7977</v>
+      </c>
+      <c r="B8" s="2" t="n">
         <v>44584</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="C8" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D8" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8" s="0" t="s">
+      <c r="D8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F8" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="G8" s="0" t="s">
+      <c r="F8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="H8" s="0" t="n">
+      <c r="H8" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="I8" s="0" t="s">
+      <c r="I8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="J8" s="0" t="s">
+      <c r="J8" s="1" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="n">
+      <c r="A9" s="1" t="n">
         <v>7977</v>
       </c>
-      <c r="B9" s="1" t="n">
+      <c r="B9" s="2" t="n">
         <v>44591</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="C9" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="E9" s="0" t="s">
+      <c r="D9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F9" s="0" t="s">
+      <c r="F9" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="G9" s="0" t="s">
+      <c r="G9" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H9" s="0" t="n">
+      <c r="H9" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="I9" s="0" t="s">
+      <c r="I9" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="J9" s="0" t="s">
+      <c r="J9" s="1" t="s">
         <v>34</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>